<commit_message>
Graficos con resultdos ejercicio 2
</commit_message>
<xml_diff>
--- a/TP2/Informe/Tiempos Mejor caso.xlsx
+++ b/TP2/Informe/Tiempos Mejor caso.xlsx
@@ -354,7 +354,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1">
         <v>1000</v>
       </c>
@@ -365,15 +365,15 @@
         <v>1000</v>
       </c>
       <c r="D1">
-        <f>5067*A1</f>
-        <v>5067000</v>
+        <f>4197*C1</f>
+        <v>4197000</v>
       </c>
       <c r="E1">
         <f>B1/A1</f>
         <v>5066.3530000000001</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>2000</v>
       </c>
@@ -384,15 +384,15 @@
         <v>2000</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D65" si="0">5067*A2</f>
-        <v>10134000</v>
+        <f t="shared" ref="D2:D65" si="0">4197*C2</f>
+        <v>8394000</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E65" si="1">B2/A2</f>
         <v>3781.1959999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>3000</v>
       </c>
@@ -404,14 +404,14 @@
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>15201000</v>
+        <v>12591000</v>
       </c>
       <c r="E3">
         <f t="shared" si="1"/>
         <v>3734.9603333333334</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>4000</v>
       </c>
@@ -423,14 +423,14 @@
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>20268000</v>
+        <v>16788000</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
         <v>3714.4740000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>5000</v>
       </c>
@@ -442,14 +442,14 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>25335000</v>
+        <v>20985000</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
         <v>3703.6030000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>6000</v>
       </c>
@@ -461,14 +461,14 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>30402000</v>
+        <v>25182000</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
         <v>3700.4703333333332</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>7000</v>
       </c>
@@ -480,14 +480,14 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>35469000</v>
+        <v>29379000</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
         <v>3750.1015714285713</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>8000</v>
       </c>
@@ -499,14 +499,18 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>40536000</v>
+        <v>33576000</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
         <v>3711.2718749999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <f>MAX(E2:E100)</f>
+        <v>4196.7811414141415</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>9000</v>
       </c>
@@ -518,14 +522,14 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>45603000</v>
+        <v>37773000</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
         <v>3702.0195555555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>10000</v>
       </c>
@@ -537,14 +541,14 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>50670000</v>
+        <v>41970000</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
         <v>3689.9535000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>11000</v>
       </c>
@@ -556,14 +560,14 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>55737000</v>
+        <v>46167000</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
         <v>3741.3570909090909</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>12000</v>
       </c>
@@ -575,14 +579,14 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>60804000</v>
+        <v>50364000</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
         <v>3752.0669166666667</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>13000</v>
       </c>
@@ -594,14 +598,14 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>65871000</v>
+        <v>54561000</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
         <v>3715.8018461538463</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>14000</v>
       </c>
@@ -613,14 +617,14 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>70938000</v>
+        <v>58758000</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
         <v>3708.4277857142856</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>15000</v>
       </c>
@@ -632,14 +636,14 @@
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>76005000</v>
+        <v>62955000</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
         <v>3717.5178666666666</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>16000</v>
       </c>
@@ -651,7 +655,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>81072000</v>
+        <v>67152000</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
@@ -670,7 +674,7 @@
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>86139000</v>
+        <v>71349000</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
@@ -689,7 +693,7 @@
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>91206000</v>
+        <v>75546000</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
@@ -708,7 +712,7 @@
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>96273000</v>
+        <v>79743000</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
@@ -727,7 +731,7 @@
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>101340000</v>
+        <v>83940000</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
@@ -746,7 +750,7 @@
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>106407000</v>
+        <v>88137000</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
@@ -765,7 +769,7 @@
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>111474000</v>
+        <v>92334000</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
@@ -784,7 +788,7 @@
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>116541000</v>
+        <v>96531000</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
@@ -803,7 +807,7 @@
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>121608000</v>
+        <v>100728000</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
@@ -822,7 +826,7 @@
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>126675000</v>
+        <v>104925000</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
@@ -841,7 +845,7 @@
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>131742000</v>
+        <v>109122000</v>
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
@@ -860,7 +864,7 @@
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>136809000</v>
+        <v>113319000</v>
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
@@ -879,7 +883,7 @@
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>141876000</v>
+        <v>117516000</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
@@ -898,7 +902,7 @@
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>146943000</v>
+        <v>121713000</v>
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
@@ -917,7 +921,7 @@
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>152010000</v>
+        <v>125910000</v>
       </c>
       <c r="E30">
         <f t="shared" si="1"/>
@@ -936,7 +940,7 @@
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>157077000</v>
+        <v>130107000</v>
       </c>
       <c r="E31">
         <f t="shared" si="1"/>
@@ -955,7 +959,7 @@
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
-        <v>162144000</v>
+        <v>134304000</v>
       </c>
       <c r="E32">
         <f t="shared" si="1"/>
@@ -974,7 +978,7 @@
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
-        <v>167211000</v>
+        <v>138501000</v>
       </c>
       <c r="E33">
         <f t="shared" si="1"/>
@@ -993,7 +997,7 @@
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>172278000</v>
+        <v>142698000</v>
       </c>
       <c r="E34">
         <f t="shared" si="1"/>
@@ -1012,7 +1016,7 @@
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
-        <v>177345000</v>
+        <v>146895000</v>
       </c>
       <c r="E35">
         <f t="shared" si="1"/>
@@ -1031,7 +1035,7 @@
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
-        <v>182412000</v>
+        <v>151092000</v>
       </c>
       <c r="E36">
         <f t="shared" si="1"/>
@@ -1050,7 +1054,7 @@
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
-        <v>187479000</v>
+        <v>155289000</v>
       </c>
       <c r="E37">
         <f t="shared" si="1"/>
@@ -1069,7 +1073,7 @@
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
-        <v>192546000</v>
+        <v>159486000</v>
       </c>
       <c r="E38">
         <f t="shared" si="1"/>
@@ -1088,7 +1092,7 @@
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
-        <v>197613000</v>
+        <v>163683000</v>
       </c>
       <c r="E39">
         <f t="shared" si="1"/>
@@ -1107,7 +1111,7 @@
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
-        <v>202680000</v>
+        <v>167880000</v>
       </c>
       <c r="E40">
         <f t="shared" si="1"/>
@@ -1126,7 +1130,7 @@
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>207747000</v>
+        <v>172077000</v>
       </c>
       <c r="E41">
         <f t="shared" si="1"/>
@@ -1145,7 +1149,7 @@
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
-        <v>212814000</v>
+        <v>176274000</v>
       </c>
       <c r="E42">
         <f t="shared" si="1"/>
@@ -1164,7 +1168,7 @@
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
-        <v>217881000</v>
+        <v>180471000</v>
       </c>
       <c r="E43">
         <f t="shared" si="1"/>
@@ -1183,7 +1187,7 @@
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
-        <v>222948000</v>
+        <v>184668000</v>
       </c>
       <c r="E44">
         <f t="shared" si="1"/>
@@ -1202,7 +1206,7 @@
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
-        <v>228015000</v>
+        <v>188865000</v>
       </c>
       <c r="E45">
         <f t="shared" si="1"/>
@@ -1221,7 +1225,7 @@
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
-        <v>233082000</v>
+        <v>193062000</v>
       </c>
       <c r="E46">
         <f t="shared" si="1"/>
@@ -1240,7 +1244,7 @@
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
-        <v>238149000</v>
+        <v>197259000</v>
       </c>
       <c r="E47">
         <f t="shared" si="1"/>
@@ -1259,7 +1263,7 @@
       </c>
       <c r="D48">
         <f t="shared" si="0"/>
-        <v>243216000</v>
+        <v>201456000</v>
       </c>
       <c r="E48">
         <f t="shared" si="1"/>
@@ -1278,7 +1282,7 @@
       </c>
       <c r="D49">
         <f t="shared" si="0"/>
-        <v>248283000</v>
+        <v>205653000</v>
       </c>
       <c r="E49">
         <f t="shared" si="1"/>
@@ -1297,7 +1301,7 @@
       </c>
       <c r="D50">
         <f t="shared" si="0"/>
-        <v>253350000</v>
+        <v>209850000</v>
       </c>
       <c r="E50">
         <f t="shared" si="1"/>
@@ -1316,7 +1320,7 @@
       </c>
       <c r="D51">
         <f t="shared" si="0"/>
-        <v>258417000</v>
+        <v>214047000</v>
       </c>
       <c r="E51">
         <f t="shared" si="1"/>
@@ -1335,7 +1339,7 @@
       </c>
       <c r="D52">
         <f t="shared" si="0"/>
-        <v>263484000</v>
+        <v>218244000</v>
       </c>
       <c r="E52">
         <f t="shared" si="1"/>
@@ -1354,7 +1358,7 @@
       </c>
       <c r="D53">
         <f t="shared" si="0"/>
-        <v>268551000</v>
+        <v>222441000</v>
       </c>
       <c r="E53">
         <f t="shared" si="1"/>
@@ -1373,7 +1377,7 @@
       </c>
       <c r="D54">
         <f t="shared" si="0"/>
-        <v>273618000</v>
+        <v>226638000</v>
       </c>
       <c r="E54">
         <f t="shared" si="1"/>
@@ -1392,7 +1396,7 @@
       </c>
       <c r="D55">
         <f t="shared" si="0"/>
-        <v>278685000</v>
+        <v>230835000</v>
       </c>
       <c r="E55">
         <f t="shared" si="1"/>
@@ -1411,7 +1415,7 @@
       </c>
       <c r="D56">
         <f t="shared" si="0"/>
-        <v>283752000</v>
+        <v>235032000</v>
       </c>
       <c r="E56">
         <f t="shared" si="1"/>
@@ -1430,7 +1434,7 @@
       </c>
       <c r="D57">
         <f t="shared" si="0"/>
-        <v>288819000</v>
+        <v>239229000</v>
       </c>
       <c r="E57">
         <f t="shared" si="1"/>
@@ -1449,7 +1453,7 @@
       </c>
       <c r="D58">
         <f t="shared" si="0"/>
-        <v>293886000</v>
+        <v>243426000</v>
       </c>
       <c r="E58">
         <f t="shared" si="1"/>
@@ -1468,7 +1472,7 @@
       </c>
       <c r="D59">
         <f t="shared" si="0"/>
-        <v>298953000</v>
+        <v>247623000</v>
       </c>
       <c r="E59">
         <f t="shared" si="1"/>
@@ -1487,7 +1491,7 @@
       </c>
       <c r="D60">
         <f t="shared" si="0"/>
-        <v>304020000</v>
+        <v>251820000</v>
       </c>
       <c r="E60">
         <f t="shared" si="1"/>
@@ -1506,7 +1510,7 @@
       </c>
       <c r="D61">
         <f t="shared" si="0"/>
-        <v>309087000</v>
+        <v>256017000</v>
       </c>
       <c r="E61">
         <f t="shared" si="1"/>
@@ -1525,7 +1529,7 @@
       </c>
       <c r="D62">
         <f t="shared" si="0"/>
-        <v>314154000</v>
+        <v>260214000</v>
       </c>
       <c r="E62">
         <f t="shared" si="1"/>
@@ -1544,7 +1548,7 @@
       </c>
       <c r="D63">
         <f t="shared" si="0"/>
-        <v>319221000</v>
+        <v>264411000</v>
       </c>
       <c r="E63">
         <f t="shared" si="1"/>
@@ -1563,7 +1567,7 @@
       </c>
       <c r="D64">
         <f t="shared" si="0"/>
-        <v>324288000</v>
+        <v>268608000</v>
       </c>
       <c r="E64">
         <f t="shared" si="1"/>
@@ -1582,7 +1586,7 @@
       </c>
       <c r="D65">
         <f t="shared" si="0"/>
-        <v>329355000</v>
+        <v>272805000</v>
       </c>
       <c r="E65">
         <f t="shared" si="1"/>
@@ -1600,8 +1604,8 @@
         <v>66000</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D100" si="2">5067*A66</f>
-        <v>334422000</v>
+        <f t="shared" ref="D66:D100" si="2">4197*C66</f>
+        <v>277002000</v>
       </c>
       <c r="E66">
         <f t="shared" ref="E66:E100" si="3">B66/A66</f>
@@ -1620,7 +1624,7 @@
       </c>
       <c r="D67">
         <f t="shared" si="2"/>
-        <v>339489000</v>
+        <v>281199000</v>
       </c>
       <c r="E67">
         <f t="shared" si="3"/>
@@ -1639,7 +1643,7 @@
       </c>
       <c r="D68">
         <f t="shared" si="2"/>
-        <v>344556000</v>
+        <v>285396000</v>
       </c>
       <c r="E68">
         <f t="shared" si="3"/>
@@ -1658,7 +1662,7 @@
       </c>
       <c r="D69">
         <f t="shared" si="2"/>
-        <v>349623000</v>
+        <v>289593000</v>
       </c>
       <c r="E69">
         <f t="shared" si="3"/>
@@ -1677,7 +1681,7 @@
       </c>
       <c r="D70">
         <f t="shared" si="2"/>
-        <v>354690000</v>
+        <v>293790000</v>
       </c>
       <c r="E70">
         <f t="shared" si="3"/>
@@ -1696,7 +1700,7 @@
       </c>
       <c r="D71">
         <f t="shared" si="2"/>
-        <v>359757000</v>
+        <v>297987000</v>
       </c>
       <c r="E71">
         <f t="shared" si="3"/>
@@ -1715,7 +1719,7 @@
       </c>
       <c r="D72">
         <f t="shared" si="2"/>
-        <v>364824000</v>
+        <v>302184000</v>
       </c>
       <c r="E72">
         <f t="shared" si="3"/>
@@ -1734,7 +1738,7 @@
       </c>
       <c r="D73">
         <f t="shared" si="2"/>
-        <v>369891000</v>
+        <v>306381000</v>
       </c>
       <c r="E73">
         <f t="shared" si="3"/>
@@ -1753,7 +1757,7 @@
       </c>
       <c r="D74">
         <f t="shared" si="2"/>
-        <v>374958000</v>
+        <v>310578000</v>
       </c>
       <c r="E74">
         <f t="shared" si="3"/>
@@ -1772,7 +1776,7 @@
       </c>
       <c r="D75">
         <f t="shared" si="2"/>
-        <v>380025000</v>
+        <v>314775000</v>
       </c>
       <c r="E75">
         <f t="shared" si="3"/>
@@ -1791,7 +1795,7 @@
       </c>
       <c r="D76">
         <f t="shared" si="2"/>
-        <v>385092000</v>
+        <v>318972000</v>
       </c>
       <c r="E76">
         <f t="shared" si="3"/>
@@ -1810,7 +1814,7 @@
       </c>
       <c r="D77">
         <f t="shared" si="2"/>
-        <v>390159000</v>
+        <v>323169000</v>
       </c>
       <c r="E77">
         <f t="shared" si="3"/>
@@ -1829,7 +1833,7 @@
       </c>
       <c r="D78">
         <f t="shared" si="2"/>
-        <v>395226000</v>
+        <v>327366000</v>
       </c>
       <c r="E78">
         <f t="shared" si="3"/>
@@ -1848,7 +1852,7 @@
       </c>
       <c r="D79">
         <f t="shared" si="2"/>
-        <v>400293000</v>
+        <v>331563000</v>
       </c>
       <c r="E79">
         <f t="shared" si="3"/>
@@ -1867,7 +1871,7 @@
       </c>
       <c r="D80">
         <f t="shared" si="2"/>
-        <v>405360000</v>
+        <v>335760000</v>
       </c>
       <c r="E80">
         <f t="shared" si="3"/>
@@ -1886,7 +1890,7 @@
       </c>
       <c r="D81">
         <f t="shared" si="2"/>
-        <v>410427000</v>
+        <v>339957000</v>
       </c>
       <c r="E81">
         <f t="shared" si="3"/>
@@ -1905,7 +1909,7 @@
       </c>
       <c r="D82">
         <f t="shared" si="2"/>
-        <v>415494000</v>
+        <v>344154000</v>
       </c>
       <c r="E82">
         <f t="shared" si="3"/>
@@ -1924,7 +1928,7 @@
       </c>
       <c r="D83">
         <f t="shared" si="2"/>
-        <v>420561000</v>
+        <v>348351000</v>
       </c>
       <c r="E83">
         <f t="shared" si="3"/>
@@ -1943,7 +1947,7 @@
       </c>
       <c r="D84">
         <f t="shared" si="2"/>
-        <v>425628000</v>
+        <v>352548000</v>
       </c>
       <c r="E84">
         <f t="shared" si="3"/>
@@ -1962,7 +1966,7 @@
       </c>
       <c r="D85">
         <f t="shared" si="2"/>
-        <v>430695000</v>
+        <v>356745000</v>
       </c>
       <c r="E85">
         <f t="shared" si="3"/>
@@ -1981,7 +1985,7 @@
       </c>
       <c r="D86">
         <f t="shared" si="2"/>
-        <v>435762000</v>
+        <v>360942000</v>
       </c>
       <c r="E86">
         <f t="shared" si="3"/>
@@ -2000,7 +2004,7 @@
       </c>
       <c r="D87">
         <f t="shared" si="2"/>
-        <v>440829000</v>
+        <v>365139000</v>
       </c>
       <c r="E87">
         <f t="shared" si="3"/>
@@ -2019,7 +2023,7 @@
       </c>
       <c r="D88">
         <f t="shared" si="2"/>
-        <v>445896000</v>
+        <v>369336000</v>
       </c>
       <c r="E88">
         <f t="shared" si="3"/>
@@ -2038,7 +2042,7 @@
       </c>
       <c r="D89">
         <f t="shared" si="2"/>
-        <v>450963000</v>
+        <v>373533000</v>
       </c>
       <c r="E89">
         <f t="shared" si="3"/>
@@ -2057,7 +2061,7 @@
       </c>
       <c r="D90">
         <f t="shared" si="2"/>
-        <v>456030000</v>
+        <v>377730000</v>
       </c>
       <c r="E90">
         <f t="shared" si="3"/>
@@ -2076,7 +2080,7 @@
       </c>
       <c r="D91">
         <f t="shared" si="2"/>
-        <v>461097000</v>
+        <v>381927000</v>
       </c>
       <c r="E91">
         <f t="shared" si="3"/>
@@ -2095,7 +2099,7 @@
       </c>
       <c r="D92">
         <f t="shared" si="2"/>
-        <v>466164000</v>
+        <v>386124000</v>
       </c>
       <c r="E92">
         <f t="shared" si="3"/>
@@ -2114,7 +2118,7 @@
       </c>
       <c r="D93">
         <f t="shared" si="2"/>
-        <v>471231000</v>
+        <v>390321000</v>
       </c>
       <c r="E93">
         <f t="shared" si="3"/>
@@ -2133,7 +2137,7 @@
       </c>
       <c r="D94">
         <f t="shared" si="2"/>
-        <v>476298000</v>
+        <v>394518000</v>
       </c>
       <c r="E94">
         <f t="shared" si="3"/>
@@ -2152,7 +2156,7 @@
       </c>
       <c r="D95">
         <f t="shared" si="2"/>
-        <v>481365000</v>
+        <v>398715000</v>
       </c>
       <c r="E95">
         <f t="shared" si="3"/>
@@ -2171,7 +2175,7 @@
       </c>
       <c r="D96">
         <f t="shared" si="2"/>
-        <v>486432000</v>
+        <v>402912000</v>
       </c>
       <c r="E96">
         <f t="shared" si="3"/>
@@ -2190,7 +2194,7 @@
       </c>
       <c r="D97">
         <f t="shared" si="2"/>
-        <v>491499000</v>
+        <v>407109000</v>
       </c>
       <c r="E97">
         <f t="shared" si="3"/>
@@ -2213,7 +2217,7 @@
       </c>
       <c r="D98">
         <f t="shared" si="2"/>
-        <v>496566000</v>
+        <v>411306000</v>
       </c>
       <c r="E98">
         <f t="shared" si="3"/>
@@ -2232,7 +2236,7 @@
       </c>
       <c r="D99">
         <f t="shared" si="2"/>
-        <v>501633000</v>
+        <v>415503000</v>
       </c>
       <c r="E99">
         <f t="shared" si="3"/>
@@ -2251,7 +2255,7 @@
       </c>
       <c r="D100">
         <f t="shared" si="2"/>
-        <v>506700000</v>
+        <v>419700000</v>
       </c>
       <c r="E100">
         <f t="shared" si="3"/>
@@ -2260,6 +2264,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>